<commit_message>
Terminado script en local, falta poner en api
</commit_message>
<xml_diff>
--- a/backend/src/data/datos.xlsx
+++ b/backend/src/data/datos.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28755" windowHeight="11655" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28755" windowHeight="11655" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="3" r:id="rId1"/>
     <sheet name="Hemocomponentes" sheetId="1" r:id="rId2"/>
     <sheet name="Pacientes" sheetId="2" r:id="rId3"/>
+    <sheet name="Pruebas" sheetId="4" r:id="rId4"/>
+    <sheet name="Transfusiones" sheetId="5" r:id="rId5"/>
+    <sheet name="EfectosAversos" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -80,6 +83,30 @@
   </si>
   <si>
     <t>AB-</t>
+  </si>
+  <si>
+    <t>hemocomponentId</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>patientId</t>
+  </si>
+  <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
+    <t>Fiebre</t>
+  </si>
+  <si>
+    <t>Muchísima fiebre</t>
   </si>
 </sst>
 </file>
@@ -411,7 +438,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +503,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -484,7 +511,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -492,7 +519,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -500,7 +527,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -508,7 +535,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -524,7 +551,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,4 +603,156 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>